<commit_message>
Update Main Gui and DB tests
</commit_message>
<xml_diff>
--- a/Notes/Notes.xlsx
+++ b/Notes/Notes.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25D3A6DF-B132-448F-A36F-12FFE118082F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +20,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Things That Need Work</t>
+  </si>
+  <si>
+    <t>The images/styles need to work</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>DB needs to be modified in order to accept login screen parameters</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,6 +85,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B838838-ECD9-4C54-A1E4-D750C8D2D96A}" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{576FB492-2695-47C5-AD7B-4DD03D5ED74D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9A060500-BDE6-4663-BA57-A6D6CE2981D8}" name="Things That Need Work"/>
+    <tableColumn id="2" xr3:uid="{51D7A399-C367-4D45-9D75-AE15311490E5}" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +360,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="60.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>